<commit_message>
Auto-committed on 2023/03/27 週一 11:43:59.62
</commit_message>
<xml_diff>
--- a/Program/Other/LM032_底稿_逾期案件滾動率明細.xlsx
+++ b/Program/Other/LM032_底稿_逾期案件滾動率明細.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>LMSAPN</t>
   </si>
@@ -65,39 +65,43 @@
     <t>科目</t>
   </si>
   <si>
+    <t>ADTYMT</t>
+  </si>
+  <si>
+    <t>GDRID1</t>
+  </si>
+  <si>
+    <t>W08PPR</t>
+  </si>
+  <si>
+    <t>LMSACN</t>
+  </si>
+  <si>
+    <t>W08LBL</t>
+  </si>
+  <si>
+    <t>ADTYMT01</t>
+  </si>
+  <si>
+    <t>GDRID101</t>
+  </si>
+  <si>
+    <t>W08PPR01</t>
+  </si>
+  <si>
+    <t>W08LBL01</t>
+  </si>
+  <si>
+    <t>戶況</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>前期年月份</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>當期年月份</t>
     <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ADTYMT</t>
-  </si>
-  <si>
-    <t>GDRID1</t>
-  </si>
-  <si>
-    <t>W08PPR</t>
-  </si>
-  <si>
-    <t>LMSACN</t>
-  </si>
-  <si>
-    <t>W08LBL</t>
-  </si>
-  <si>
-    <t>ADTYMT01</t>
-  </si>
-  <si>
-    <t>GDRID101</t>
-  </si>
-  <si>
-    <t>W08PPR01</t>
-  </si>
-  <si>
-    <t>W08LBL01</t>
   </si>
 </sst>
 </file>
@@ -106,7 +110,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="#,##0_);[Red]\(#,##0\)"/>
+    <numFmt numFmtId="176" formatCode="#,##0_);[Red]\(#,##0\)"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -745,9 +749,9 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="22" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="178" fontId="24" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="178" fontId="23" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="22" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="24" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="23" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
@@ -1105,7 +1109,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17"/>
@@ -1128,55 +1132,54 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="P1"/>
     </row>
     <row r="2" spans="1:16" s="2" customFormat="1">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
@@ -1196,9 +1199,11 @@
       <c r="G2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="5"/>
+      <c r="H2" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="I2" s="3" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>7</v>

</xml_diff>